<commit_message>
delete stages and add cv to index
</commit_message>
<xml_diff>
--- a/fichiers/tableauSyntheseE5.xlsx
+++ b/fichiers/tableauSyntheseE5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\portfolio\fichiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B439B8FC-8682-4D93-AF85-5A3C34208F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC811CF3-D0E1-4F35-9B27-C2575A48BC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,9 +180,6 @@
     <t>02/12/2024 - 10/12/2024</t>
   </si>
   <si>
-    <t>11/12/2024 - ?</t>
-  </si>
-  <si>
     <t>projet création de site web : Les Paniers Gourmands</t>
   </si>
   <si>
@@ -229,6 +226,9 @@
   </si>
   <si>
     <t>Adresse URL du portfolio : http://localhost/portfolio/</t>
+  </si>
+  <si>
+    <t>11/12/2024 - 16/01/25</t>
   </si>
 </sst>
 </file>
@@ -763,9 +763,36 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -777,33 +804,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1116,8 +1116,8 @@
   </sheetPr>
   <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1130,56 +1130,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="34"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="35" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="37"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="46"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="28" t="s">
         <v>6</v>
       </c>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
@@ -1203,10 +1203,10 @@
       <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="42" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="25" t="s">
@@ -1229,8 +1229,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="47"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="16" t="s">
         <v>17</v>
       </c>
@@ -1286,16 +1286,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="42"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1334,22 +1334,22 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="49.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="21"/>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>26</v>
@@ -1408,7 +1408,7 @@
         <v>24</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>27</v>
@@ -1833,16 +1833,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="45"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="41"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>31</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>32</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>35</v>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="24">
         <v>45475</v>
@@ -2241,16 +2241,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="45"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="41"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2289,7 +2289,7 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>37</v>
@@ -2348,10 +2348,10 @@
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7" t="s">
@@ -2454,10 +2454,10 @@
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>53</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -2507,10 +2507,10 @@
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7" t="s">
@@ -2876,17 +2876,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>